<commit_message>
Added formulas to result table
</commit_message>
<xml_diff>
--- a/toolkit/debug/auto_well_data/sheets/WMOCNewFormattest1.xlsx
+++ b/toolkit/debug/auto_well_data/sheets/WMOCNewFormattest1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\Desktop\programming\Python\FGCU-HG-Toolkit\toolkit\debug\auto_well_data\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E78CEF8-1FE3-4AFD-B38A-7D6B0FB97512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF953A9A-A433-49E4-A161-C27F53753CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="345" yWindow="2790" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -282,7 +282,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="m/d/yy"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -368,6 +368,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -401,7 +406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -469,8 +474,9 @@
     <xf numFmtId="18" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5244,19 +5250,19 @@
     </row>
     <row r="3" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14">
-        <f t="shared" ref="A3:A13" si="0">G3</f>
+        <f t="shared" ref="A3:A14" si="0">G3</f>
         <v>44266</v>
       </c>
       <c r="B3" s="15">
-        <f t="shared" ref="B3:B13" si="1">H3</f>
+        <f t="shared" ref="B3:B14" si="1">H3</f>
         <v>0.37847222222222221</v>
       </c>
       <c r="C3" s="19">
-        <f t="shared" ref="C3:C13" si="2">D3/305</f>
+        <f t="shared" ref="C3:C14" si="2">D3/305</f>
         <v>6.1400000000000006</v>
       </c>
       <c r="D3" s="19">
-        <f t="shared" ref="D3:D13" si="3">I3</f>
+        <f t="shared" ref="D3:D14" si="3">I3</f>
         <v>1872.7</v>
       </c>
       <c r="E3" s="19">
@@ -5546,7 +5552,7 @@
         <v>0.40208333333333329</v>
       </c>
       <c r="C13" s="19">
-        <f t="shared" si="2"/>
+        <f>D13/305</f>
         <v>6.71</v>
       </c>
       <c r="D13" s="19">
@@ -5564,15 +5570,15 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="31"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="28"/>
-      <c r="C14" s="26"/>
+      <c r="C14" s="33"/>
       <c r="D14" s="26"/>
       <c r="G14" s="29"/>
       <c r="H14" s="30"/>
     </row>
     <row r="15" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="32"/>
+      <c r="A15" s="31"/>
     </row>
     <row r="16" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Set correct number format
</commit_message>
<xml_diff>
--- a/toolkit/debug/auto_well_data/sheets/WMOCNewFormattest1.xlsx
+++ b/toolkit/debug/auto_well_data/sheets/WMOCNewFormattest1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\Desktop\programming\Python\FGCU-HG-Toolkit\toolkit\debug\auto_well_data\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF953A9A-A433-49E4-A161-C27F53753CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E297E45E-5E3E-4D9D-8101-1A1105686C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="2790" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4590" yWindow="3210" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All Wells" sheetId="1" r:id="rId1"/>
@@ -5204,7 +5204,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="A14" sqref="A14:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5552,7 +5552,7 @@
         <v>0.40208333333333329</v>
       </c>
       <c r="C13" s="19">
-        <f>D13/305</f>
+        <f t="shared" si="2"/>
         <v>6.71</v>
       </c>
       <c r="D13" s="19">

</xml_diff>

<commit_message>
Setting up sheet dropdown
</commit_message>
<xml_diff>
--- a/toolkit/debug/auto_well_data/sheets/WMOCNewFormattest1.xlsx
+++ b/toolkit/debug/auto_well_data/sheets/WMOCNewFormattest1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\Desktop\programming\Python\FGCU-HG-Toolkit\toolkit\debug\auto_well_data\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{709DD58F-2162-4690-957C-A140C278316E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57706369-C13A-45C1-AEFF-52616B81F6C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4590" yWindow="3210" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5204,7 +5204,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:I14"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>